<commit_message>
dialogue and quest to static renewal
</commit_message>
<xml_diff>
--- a/Assets/02Script/Manager/QuestManager/QuestSheet.xlsx
+++ b/Assets/02Script/Manager/QuestManager/QuestSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JSK\Desktop\UnityGames\RPGGame\Assets\02Script\Manager\QuestManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4C0BD5-857D-45BD-89FE-A607A7232F12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8C8C4E-2E3A-496D-9275-640509E52973}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="1635" windowWidth="21600" windowHeight="11385" xr2:uid="{0CF11EFC-30A0-4706-A078-CD6AEDF13D6B}"/>
+    <workbookView xWindow="1365" yWindow="3900" windowWidth="21600" windowHeight="11385" xr2:uid="{0CF11EFC-30A0-4706-A078-CD6AEDF13D6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,34 +35,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>needItem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>needCount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>길버트</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>rewardItem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rewardCount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>5;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -79,7 +55,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>dialogueIndex</t>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DialogueIndex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NeedItem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NeedCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardItem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardCount</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -447,7 +447,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -460,30 +460,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -492,16 +492,16 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -512,21 +512,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x01010023ABF18EEC8FEC4B8EEB286042C6FC34" ma:contentTypeVersion="7" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="0145b38d72a31460beff979789b4c23d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bcb34f15-5958-4dad-9098-949b92181baa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffd077ba9f193c42eb3b9c001ddbb664" ns3:_="">
     <xsd:import namespace="bcb34f15-5958-4dad-9098-949b92181baa"/>
@@ -690,24 +675,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32474EF9-E52C-4F04-B55B-0C9726A9FFF9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742BBA78-C0C9-4230-A372-EA79AEE7624F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{226C2612-2DA0-414B-8C56-CB556EF0F531}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -723,4 +706,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742BBA78-C0C9-4230-A372-EA79AEE7624F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32474EF9-E52C-4F04-B55B-0C9726A9FFF9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
dialogue and quest renewal 1.0
</commit_message>
<xml_diff>
--- a/Assets/02Script/Manager/QuestManager/QuestSheet.xlsx
+++ b/Assets/02Script/Manager/QuestManager/QuestSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JSK\Desktop\UnityGames\RPGGame\Assets\02Script\Manager\QuestManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SungyuJang\Desktop\GitHubDesktop\RPGGame\Assets\02Script\Manager\QuestManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8C8C4E-2E3A-496D-9275-640509E52973}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B553D894-D010-496C-9BFC-32A5DB8E5B25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="3900" windowWidth="21600" windowHeight="11385" xr2:uid="{0CF11EFC-30A0-4706-A078-CD6AEDF13D6B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0CF11EFC-30A0-4706-A078-CD6AEDF13D6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -489,7 +489,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -512,6 +512,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x01010023ABF18EEC8FEC4B8EEB286042C6FC34" ma:contentTypeVersion="7" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="0145b38d72a31460beff979789b4c23d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bcb34f15-5958-4dad-9098-949b92181baa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffd077ba9f193c42eb3b9c001ddbb664" ns3:_="">
     <xsd:import namespace="bcb34f15-5958-4dad-9098-949b92181baa"/>
@@ -675,22 +690,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32474EF9-E52C-4F04-B55B-0C9726A9FFF9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742BBA78-C0C9-4230-A372-EA79AEE7624F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{226C2612-2DA0-414B-8C56-CB556EF0F531}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -706,21 +723,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742BBA78-C0C9-4230-A372-EA79AEE7624F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32474EF9-E52C-4F04-B55B-0C9726A9FFF9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
inventoryView and ItemView Fixed
itemView create by itemManager for QuestManager.

itemView handle by itemManager.
</commit_message>
<xml_diff>
--- a/Assets/02Script/Manager/QuestManager/QuestSheet.xlsx
+++ b/Assets/02Script/Manager/QuestManager/QuestSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SungyuJang\Desktop\GitHubDesktop\RPGGame\Assets\02Script\Manager\QuestManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jang\Desktop\GitHubGameProject\RPGGame\Assets\02Script\Manager\QuestManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B553D894-D010-496C-9BFC-32A5DB8E5B25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A53C54-B2C0-452A-A1FE-994F6DF1CB84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0CF11EFC-30A0-4706-A078-CD6AEDF13D6B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CF11EFC-30A0-4706-A078-CD6AEDF13D6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>길버트</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,6 +80,22 @@
   </si>
   <si>
     <t>RewardCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>길버트에게 오래된 동전을 가져다주자.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>길버트 아저씨가 도와달라 한다. \r\n 얻어먹은 것도 있으니 일단은 노력해보자.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -444,21 +460,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E1FA90-6EF9-4267-B485-7B9D066C34F4}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.625" customWidth="1"/>
-    <col min="5" max="6" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -469,19 +487,25 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -492,15 +516,21 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>